<commit_message>
markerpdf fro pdf text extraction
</commit_message>
<xml_diff>
--- a/reports/experiments.xlsx
+++ b/reports/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\vpp-cfla\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B622C5D7-4728-4139-A357-0F1C58D1DC1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F22E534-DD08-46C2-A492-996D26A837B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -97,12 +97,15 @@
   <si>
     <t>mainītas uzvednes un jautājumi</t>
   </si>
+  <si>
+    <t>chunk_size = 1536, MammothMarkdownify,Markerpdf, JSON rezultāts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +129,13 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="186"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,12 +157,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,6 +802,26 @@
         <v>18</v>
       </c>
     </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.52682926829268295</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Previouse/next chunk for the similar chunk
</commit_message>
<xml_diff>
--- a/reports/experiments.xlsx
+++ b/reports/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\vpp-cfla\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB171D1-84AC-42FE-8A61-81D336CACD24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D03508-93AF-48AF-A6DB-344EBF75A71F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Viss fails tiek padots LLMam</t>
-  </si>
-  <si>
-    <t>reranker, chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
   </si>
   <si>
     <r>
@@ -185,6 +182,24 @@
 25. Ir izgūts nolikuma numurs. Pareizi saka, ka "nav informācijas par to, vai šis numurs ir tāds pats kā publikācijā IUB".
 29. TIkai viss dokuments konstatē, ka piedāvājumā ir piedāvājumu iesniegšanas termiņš. To vajag izgūt. Papildu darība - salīdzināt ar paziņojumu par līgumu</t>
     </r>
+  </si>
+  <si>
+    <t>5 top similar, prevchunk,similar chunk, nextchunk,chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
+  </si>
+  <si>
+    <t>5 top similar, chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
+  </si>
+  <si>
+    <t>20 reranker, 5 top similar,  chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
+  </si>
+  <si>
+    <t>3 top similar, prevchunk,similar chunk, nextchunk,chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
+  </si>
+  <si>
+    <t>4 top similar, prevchunk,similar chunk, nextchunk,chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
+  </si>
+  <si>
+    <t>20 reranker, 5 top similar, prevchunk,similar chunk, nextchunk,chunk_size = 1536, MammothMarkdownify, JSON rezultāts</t>
   </si>
 </sst>
 </file>
@@ -331,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -368,6 +383,7 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -657,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,8 +1128,8 @@
       <c r="F22" s="9">
         <v>0.55609756097560903</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>22</v>
+      <c r="G22" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1130,12 +1146,12 @@
         <v>6</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F23" s="13">
         <v>0.46341463414634099</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
@@ -1151,12 +1167,92 @@
         <v>6</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F24" s="17">
         <v>0.45853658536585301</v>
       </c>
-      <c r="G24" s="20"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>27.05</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.54146341463414605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <v>27.05</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.517073170731707</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>27.05</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.482926829268292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <v>27.05</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.56097560975609695</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>